<commit_message>
questao 1 e 2 com os 5 metodos
</commit_message>
<xml_diff>
--- a/cálculo numérico/atividade 1/metodos.xlsx
+++ b/cálculo numérico/atividade 1/metodos.xlsx
@@ -473,20 +473,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a=1.0, b=2.0, ε=0.0001</t>
+          <t>a=1.0, b=2.0, ε=1e-06</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.44741821</v>
+        <v>1.324718</v>
       </c>
       <c r="D2" t="n">
-        <v>2.50738811e-06</v>
+        <v>1.75958307e-07</v>
       </c>
       <c r="E2" t="n">
-        <v>6.10351562e-05</v>
+        <v>9.53674316e-07</v>
       </c>
       <c r="F2" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -497,20 +497,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a=1.0, b=2.0, ε=0.0001</t>
+          <t>a=1.0, b=2.0, ε=1e-06</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1.44740335</v>
+        <v>1.32471787</v>
       </c>
       <c r="D3" t="n">
-        <v>-6.94767402e-06</v>
+        <v>-3.51552278e-07</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -521,17 +521,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>x0=1.2, ε=0.0001</t>
+          <t>x0=1.2, ε=1e-06</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.44728118</v>
+        <v>1.32471774</v>
       </c>
       <c r="D4" t="n">
-        <v>-8.46549312e-05</v>
+        <v>-9.21852971e-07</v>
       </c>
       <c r="E4" t="n">
-        <v>0.000232509201</v>
+        <v>9.21852971e-07</v>
       </c>
       <c r="F4" t="n">
         <v>8</v>
@@ -545,20 +545,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>x0=1.2, ε=0.0001</t>
+          <t>x0=0.5, ε=1e-06</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.4474335</v>
+        <v>1.324718</v>
       </c>
       <c r="D5" t="n">
-        <v>1.22319516e-05</v>
+        <v>1.74374144e-07</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0052084024</v>
+        <v>0.000209457449</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -569,26 +569,24 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>x0=1.0, x1=2.0, ε=0.0001</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1.44741345</t>
-        </is>
+          <t>x0=0.0, x1=0.5, ε=1e-06</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1.32471795</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>-5.24224992e-7</t>
+          <t>-4.34057552e-08</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.85528948e-4</t>
+          <t>1.19166137e-05</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>